<commit_message>
more doc, web intro, style changes
</commit_message>
<xml_diff>
--- a/doc/presupuesto.xlsx
+++ b/doc/presupuesto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Unidades de trabajo" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>PRESUPUESTO DE EJECUCION DE MATERIAL</t>
   </si>
   <si>
-    <t>Beneficios (20%)</t>
-  </si>
-  <si>
     <t>PRESUPUESTO DE EJECUCIÓN</t>
   </si>
   <si>
@@ -255,6 +252,9 @@
   </si>
   <si>
     <t>Desarrollo web</t>
+  </si>
+  <si>
+    <t>Beneficios (30%)</t>
   </si>
 </sst>
 </file>
@@ -630,24 +630,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -665,6 +647,25 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -677,7 +678,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,18 +1046,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="G2" s="41" t="s">
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="G2" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1148,15 +1148,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="51" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1243,10 +1243,10 @@
       <c r="B7" s="11"/>
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="42"/>
+      <c r="F7" s="52"/>
       <c r="G7" s="13">
         <f>F5+F6</f>
         <v>19.350000000000001</v>
@@ -1257,10 +1257,10 @@
       <c r="B8" s="11"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
-      <c r="E8" s="43" t="s">
+      <c r="E8" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="43"/>
+      <c r="F8" s="53"/>
       <c r="G8" s="14">
         <f>G7*8</f>
         <v>154.80000000000001</v>
@@ -1365,10 +1365,10 @@
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
       <c r="D15" s="11"/>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="42"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="17">
         <f>F13+F14</f>
         <v>13.49</v>
@@ -1379,10 +1379,10 @@
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="43"/>
+      <c r="F16" s="53"/>
       <c r="G16" s="18">
         <f>G15*8</f>
         <v>107.92</v>
@@ -1404,8 +1404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,12 +1415,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D3" s="19"/>
@@ -1429,11 +1429,11 @@
       <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1486,11 +1486,11 @@
       <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="C11" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
@@ -1540,11 +1540,11 @@
       <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="44" t="s">
+      <c r="C17" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
@@ -1562,7 +1562,7 @@
     </row>
     <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>48</v>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="E19" s="5">
         <f>B19*D19</f>
-        <v>599.85</v>
+        <v>638.55000000000007</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="E20" s="5">
         <f>SUM(E16:E19)</f>
-        <v>599.85</v>
+        <v>638.55000000000007</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1594,11 +1594,11 @@
       <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="44" t="s">
+      <c r="C23" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="55"/>
     </row>
     <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
@@ -1616,7 +1616,7 @@
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>34.200000000000003</v>
+        <v>37</v>
       </c>
       <c r="C25" s="20" t="s">
         <v>48</v>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="E25" s="5">
         <f>B25*D25</f>
-        <v>661.7700000000001</v>
+        <v>715.95</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -1635,7 +1635,7 @@
       </c>
       <c r="E26" s="5">
         <f>SUM(E24:E25)</f>
-        <v>661.7700000000001</v>
+        <v>715.95</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -1651,11 +1651,11 @@
       <c r="B30" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="44" t="s">
+      <c r="C30" s="54" t="s">
         <v>49</v>
       </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
@@ -1708,11 +1708,11 @@
       <c r="B37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="44" t="s">
+      <c r="C37" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
+      <c r="D37" s="55"/>
+      <c r="E37" s="55"/>
     </row>
     <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
@@ -1730,7 +1730,7 @@
     </row>
     <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="3">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>22</v>
@@ -1740,7 +1740,7 @@
       </c>
       <c r="E39" s="5">
         <f>B39*D39</f>
-        <v>133.9</v>
+        <v>200.85000000000002</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
@@ -1749,18 +1749,18 @@
       </c>
       <c r="E40" s="5">
         <f>SUM(E36:E39)</f>
-        <v>133.9</v>
+        <v>200.85000000000002</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="44" t="s">
+      <c r="C43" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="55"/>
     </row>
     <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
@@ -1778,7 +1778,7 @@
     </row>
     <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="3">
-        <v>6.83</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>22</v>
@@ -1788,7 +1788,7 @@
       </c>
       <c r="E45" s="5">
         <f>B45*D45</f>
-        <v>91.453699999999998</v>
+        <v>116.49299999999999</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
@@ -1797,18 +1797,18 @@
       </c>
       <c r="E46" s="5">
         <f>SUM(E42:E45)</f>
-        <v>91.453699999999998</v>
+        <v>116.49299999999999</v>
       </c>
     </row>
     <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C49" s="44" t="s">
+      <c r="C49" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="55"/>
     </row>
     <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="6" t="s">
@@ -1826,7 +1826,7 @@
     </row>
     <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="3">
-        <v>18.329999999999998</v>
+        <v>24.6</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>22</v>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="E51" s="5">
         <f>B51*D51</f>
-        <v>245.43869999999998</v>
+        <v>329.39400000000001</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
@@ -1845,18 +1845,18 @@
       </c>
       <c r="E52" s="5">
         <f>SUM(E48:E51)</f>
-        <v>245.43869999999998</v>
+        <v>329.39400000000001</v>
       </c>
     </row>
     <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C55" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="C55" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
+      <c r="D55" s="55"/>
+      <c r="E55" s="55"/>
     </row>
     <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
@@ -1918,7 +1918,7 @@
   <dimension ref="A2:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,12 +1929,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -1943,118 +1943,127 @@
       <c r="B3" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="59"/>
+      <c r="D3" s="60"/>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="C4" s="56">
-        <v>338.63</v>
-      </c>
-      <c r="D4" s="57"/>
+        <v>60</v>
+      </c>
+      <c r="C4" s="57">
+        <f>'Precios de unidades de obra'!E7</f>
+        <v>338.625</v>
+      </c>
+      <c r="D4" s="58"/>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="56">
+        <v>61</v>
+      </c>
+      <c r="C5" s="57">
+        <f>'Precios de unidades de obra'!E14</f>
         <v>96.75</v>
       </c>
-      <c r="D5" s="57"/>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="56">
-        <v>599.85</v>
-      </c>
-      <c r="D6" s="57"/>
+        <v>62</v>
+      </c>
+      <c r="C6" s="57">
+        <f>'Precios de unidades de obra'!E20</f>
+        <v>638.55000000000007</v>
+      </c>
+      <c r="D6" s="58"/>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="56">
-        <v>661.77</v>
-      </c>
-      <c r="D7" s="57"/>
+        <v>63</v>
+      </c>
+      <c r="C7" s="57">
+        <f>'Precios de unidades de obra'!E26</f>
+        <v>715.95</v>
+      </c>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="56">
+        <v>64</v>
+      </c>
+      <c r="C8" s="57">
+        <f>'Precios de unidades de obra'!E33</f>
         <v>290.25</v>
       </c>
-      <c r="D8" s="57"/>
+      <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="56">
-        <v>133.9</v>
-      </c>
-      <c r="D9" s="57"/>
+        <v>65</v>
+      </c>
+      <c r="C9" s="57">
+        <f>'Precios de unidades de obra'!E40</f>
+        <v>200.85000000000002</v>
+      </c>
+      <c r="D9" s="58"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="56">
-        <v>91.45</v>
-      </c>
-      <c r="D10" s="57"/>
+        <v>66</v>
+      </c>
+      <c r="C10" s="57">
+        <f>'Precios de unidades de obra'!E46</f>
+        <v>116.49299999999999</v>
+      </c>
+      <c r="D10" s="58"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="56">
-        <v>245.44</v>
-      </c>
-      <c r="D11" s="57"/>
+        <v>67</v>
+      </c>
+      <c r="C11" s="57">
+        <f>'Precios de unidades de obra'!E52</f>
+        <v>329.39400000000001</v>
+      </c>
+      <c r="D11" s="58"/>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="56">
+        <v>68</v>
+      </c>
+      <c r="C12" s="57">
+        <f>'Precios de unidades de obra'!E58</f>
         <v>13.39</v>
       </c>
-      <c r="D12" s="57"/>
+      <c r="D12" s="58"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
@@ -2064,20 +2073,20 @@
       </c>
       <c r="D13" s="27">
         <f>SUM(C4:D12)</f>
-        <v>2471.4299999999998</v>
+        <v>2740.252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>56</v>
       </c>
       <c r="D14" s="31">
         <f>D13*0.1</f>
-        <v>247.143</v>
+        <v>274.02519999999998</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -2088,29 +2097,29 @@
       </c>
       <c r="D15" s="34">
         <f>D13+D14</f>
-        <v>2718.5729999999999</v>
+        <v>3014.2772</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="35"/>
       <c r="C16" s="29" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="D16" s="36">
-        <f>D13*0.2</f>
-        <v>494.286</v>
+        <f>D13*0.3</f>
+        <v>822.07560000000001</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="38"/>
       <c r="C17" s="39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="40">
         <f>D15+D16</f>
-        <v>3212.8589999999999</v>
+        <v>3836.3528000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2136,7 +2145,7 @@
   <dimension ref="B3:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2147,69 +2156,69 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="41"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="43">
+        <f>SUM('Presupuesto Interno'!C4:D8)*1.4</f>
+        <v>2912.1749999999997</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="43">
+        <f>SUM('Presupuesto Interno'!C9:D12)*1.4</f>
+        <v>924.17780000000005</v>
+      </c>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B7" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="47"/>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="48"/>
-      <c r="C4" s="48"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="49">
-        <f>SUM('Presupuesto Interno'!C4:D8)*1.3</f>
-        <v>2583.4250000000002</v>
-      </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="49">
-        <f>SUM('Presupuesto Interno'!C9:D12)*1.3</f>
-        <v>629.43400000000008</v>
-      </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-    </row>
-    <row r="7" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B7" s="50" t="s">
+      <c r="C7" s="45">
+        <f>SUM(C5:C6)</f>
+        <v>3836.3527999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="51">
-        <f>SUM(C5:C6)</f>
-        <v>3212.8590000000004</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="52" t="s">
+      <c r="C8" s="47">
+        <f>C7*0.21</f>
+        <v>805.63408799999991</v>
+      </c>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="53">
-        <f>C7*0.21</f>
-        <v>674.70039000000008</v>
-      </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-    </row>
-    <row r="9" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="55">
+      <c r="C9" s="49">
         <f>C7+C8</f>
-        <v>3887.5593900000003</v>
+        <v>4641.9868879999995</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
More doc. Remaining: Use cases extended, tests, manual.
</commit_message>
<xml_diff>
--- a/doc/presupuesto.xlsx
+++ b/doc/presupuesto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Unidades de trabajo" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="77">
   <si>
     <t>Análisis de lenguaje natural</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Aprendizaje</t>
   </si>
   <si>
-    <t>Asiganción temas</t>
-  </si>
-  <si>
     <t>Web</t>
   </si>
   <si>
@@ -83,15 +80,9 @@
     <t>h</t>
   </si>
   <si>
-    <t>Diseñador gráfico</t>
-  </si>
-  <si>
     <t>RP2</t>
   </si>
   <si>
-    <t>Desarrollador con conocimientos de IA</t>
-  </si>
-  <si>
     <t>Desarrollador web</t>
   </si>
   <si>
@@ -122,9 +113,6 @@
     <t>Importe diario</t>
   </si>
   <si>
-    <t>Coste del desarrollador IA</t>
-  </si>
-  <si>
     <t>Coste del desarrollador web</t>
   </si>
   <si>
@@ -170,9 +158,6 @@
     <t>Recopilación textos</t>
   </si>
   <si>
-    <t>Desarrollador IA</t>
-  </si>
-  <si>
     <t>Resultados y asignación</t>
   </si>
   <si>
@@ -233,9 +218,6 @@
     <t>Precio nº9: Validación</t>
   </si>
   <si>
-    <t>(10% del costo del proyecto)</t>
-  </si>
-  <si>
     <t>PRESUPUESTO EXTERNO</t>
   </si>
   <si>
@@ -255,6 +237,24 @@
   </si>
   <si>
     <t>Beneficios (30%)</t>
+  </si>
+  <si>
+    <t>Historiador</t>
+  </si>
+  <si>
+    <t>RP3</t>
+  </si>
+  <si>
+    <t>Coste del historiador</t>
+  </si>
+  <si>
+    <t>(17% del costo del proyecto)</t>
+  </si>
+  <si>
+    <t>Experto en análisis de lenguaje</t>
+  </si>
+  <si>
+    <t>Coste del experto en análisis del lenguaje</t>
   </si>
 </sst>
 </file>
@@ -264,7 +264,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +354,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -536,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,6 +684,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,7 +971,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,32 +1003,32 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1029,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J5"/>
+  <dimension ref="A2:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="G3" sqref="G3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,13 +1057,13 @@
   <sheetData>
     <row r="2" spans="1:10" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
       <c r="D2" s="51"/>
       <c r="G2" s="51" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2" s="51"/>
       <c r="I2" s="51"/>
@@ -1061,51 +1071,51 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="5">
+        <v>25.2</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="5">
-        <v>19.25</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J4" s="5">
         <v>0.1</v>
@@ -1113,16 +1123,30 @@
     </row>
     <row r="5" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5">
-        <v>13.39</v>
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="5">
+        <v>17.399999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -1136,20 +1160,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G16"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="51" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -1160,73 +1184,75 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="7" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>19</v>
+      <c r="C5" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="D5" s="5">
-        <v>19.25</v>
+        <f>'Precios básicos'!D4</f>
+        <v>25.2</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="10">
         <f>D5*E5</f>
-        <v>19.25</v>
+        <v>25.2</v>
       </c>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="5">
+        <f>'Precios básicos'!J4</f>
         <v>0.1</v>
       </c>
       <c r="E6" s="3">
@@ -1244,12 +1270,12 @@
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
       <c r="E7" s="52" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F7" s="52"/>
       <c r="G7" s="13">
         <f>F5+F6</f>
-        <v>19.350000000000001</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1258,12 +1284,12 @@
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
       <c r="E8" s="53" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F8" s="53"/>
       <c r="G8" s="14">
         <f>G7*8</f>
-        <v>154.80000000000001</v>
+        <v>202.4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1282,34 +1308,34 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="16"/>
@@ -1318,37 +1344,39 @@
     </row>
     <row r="13" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D13" s="5">
-        <v>13.39</v>
+        <f>'Precios básicos'!D5</f>
+        <v>16.399999999999999</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="5">
         <f>D13*E13</f>
-        <v>13.39</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="G13" s="8"/>
     </row>
     <row r="14" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="5">
+        <f>'Precios básicos'!J4</f>
         <v>0.1</v>
       </c>
       <c r="E14" s="3">
@@ -1366,12 +1394,12 @@
       <c r="C15" s="12"/>
       <c r="D15" s="11"/>
       <c r="E15" s="52" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F15" s="52"/>
       <c r="G15" s="17">
         <f>F13+F14</f>
-        <v>13.49</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1380,16 +1408,127 @@
       <c r="C16" s="12"/>
       <c r="D16" s="11"/>
       <c r="E16" s="53" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F16" s="53"/>
       <c r="G16" s="18">
         <f>G15*8</f>
-        <v>107.92</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="5">
+        <f>'Precios básicos'!D6</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="E21" s="3">
+        <v>1</v>
+      </c>
+      <c r="F21" s="5">
+        <f>D21*E21</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="3">
+        <v>1</v>
+      </c>
+      <c r="F22" s="10">
+        <f>D22*E22</f>
+        <v>0.1</v>
+      </c>
+      <c r="G22" s="8"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="52" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="52"/>
+      <c r="G23" s="17">
+        <f>F21+F22</f>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="53"/>
+      <c r="G24" s="18">
+        <f>G23*8</f>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
@@ -1402,21 +1541,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E58"/>
+  <dimension ref="B2:E60"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57:E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B2" s="56" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C2" s="56"/>
       <c r="D2" s="56"/>
@@ -1427,50 +1566,50 @@
     </row>
     <row r="4" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D4" s="55"/>
       <c r="E4" s="55"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B6" s="20">
-        <v>17.5</v>
-      </c>
-      <c r="C6" s="20" t="s">
-        <v>48</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="61" t="s">
+        <v>75</v>
       </c>
       <c r="D6" s="21">
-        <v>19.350000000000001</v>
+        <v>25.3</v>
       </c>
       <c r="E6" s="21">
         <f>D6*B6</f>
-        <v>338.625</v>
+        <v>455.40000000000003</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D7" s="22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E7" s="5">
         <f>SUM(E5:E6)</f>
-        <v>338.625</v>
+        <v>455.40000000000003</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -1484,7 +1623,7 @@
     </row>
     <row r="11" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C11" s="54" t="s">
         <v>2</v>
@@ -1494,40 +1633,40 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
-        <v>5</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>48</v>
+        <v>8</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>75</v>
       </c>
       <c r="D13" s="21">
-        <v>19.350000000000001</v>
+        <v>25.3</v>
       </c>
       <c r="E13" s="5">
         <f>B13*D13</f>
-        <v>96.75</v>
+        <v>202.4</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D14" s="22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5">
         <f>SUM(E11:E13)</f>
-        <v>96.75</v>
+        <v>202.4</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
@@ -1538,7 +1677,7 @@
     </row>
     <row r="17" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C17" s="54" t="s">
         <v>3</v>
@@ -1548,40 +1687,41 @@
     </row>
     <row r="18" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B19" s="3">
+        <f>17+8*3</f>
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
-        <v>33</v>
-      </c>
-      <c r="C19" s="20" t="s">
-        <v>48</v>
+      <c r="C19" s="61" t="s">
+        <v>75</v>
       </c>
       <c r="D19" s="21">
-        <v>19.350000000000001</v>
+        <v>25.3</v>
       </c>
       <c r="E19" s="5">
         <f>B19*D19</f>
-        <v>638.55000000000007</v>
+        <v>1037.3</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D20" s="22" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E20" s="5">
         <f>SUM(E16:E19)</f>
-        <v>638.55000000000007</v>
+        <v>1037.3</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
@@ -1592,7 +1732,7 @@
     </row>
     <row r="23" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C23" s="54" t="s">
         <v>4</v>
@@ -1602,44 +1742,58 @@
     </row>
     <row r="24" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="3">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D25" s="21">
-        <v>19.350000000000001</v>
+        <f>'Costes unitarios'!G23</f>
+        <v>17.5</v>
       </c>
       <c r="E25" s="5">
         <f>B25*D25</f>
-        <v>715.95</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="22" t="s">
-        <v>41</v>
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <f>5.2+2+3+2+1+0.5+4+2+1.5+1+0.5+1.5+3+2+0.5+2+2+0.5+8+1+8+1+30+1</f>
+        <v>83.2</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="21">
+        <v>25.3</v>
       </c>
       <c r="E26" s="5">
-        <f>SUM(E24:E25)</f>
-        <v>715.95</v>
+        <f>B26*D26</f>
+        <v>2104.96</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D27" s="19"/>
+      <c r="D27" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="5">
+        <f>SUM(E24:E26)</f>
+        <v>2122.46</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D28" s="19"/>
@@ -1647,269 +1801,295 @@
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D29" s="19"/>
     </row>
-    <row r="30" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="55"/>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="19"/>
     </row>
     <row r="31" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E31" s="6" t="s">
+      <c r="B31" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="C31" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
     </row>
     <row r="32" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="3">
-        <v>15</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="21">
-        <v>19.350000000000001</v>
-      </c>
-      <c r="E32" s="5">
-        <f>B32*D32</f>
-        <v>290.25</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D33" s="22" t="s">
-        <v>41</v>
+      <c r="B32" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="3">
+        <f>4*8</f>
+        <v>32</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="21">
+        <f>'Costes unitarios'!G23</f>
+        <v>17.5</v>
       </c>
       <c r="E33" s="5">
-        <f>SUM(E29:E32)</f>
-        <v>290.25</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D34" s="19"/>
+        <f>B33*D33</f>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B34" s="3">
+        <f>4*8</f>
+        <v>32</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="21">
+        <f>'Costes unitarios'!G7</f>
+        <v>25.3</v>
+      </c>
+      <c r="E34" s="5">
+        <f>B34*D34</f>
+        <v>809.6</v>
+      </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D35" s="19"/>
+      <c r="D35" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E35" s="5">
+        <f>SUM(E30:E34)</f>
+        <v>1369.6</v>
+      </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D36" s="19"/>
     </row>
-    <row r="37" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="2" t="s">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D37" s="19"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D38" s="19"/>
+    </row>
+    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="55"/>
+      <c r="E39" s="55"/>
+    </row>
+    <row r="40" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="3">
+        <f>4.5*8</f>
+        <v>36</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="21">
+        <v>13.39</v>
+      </c>
+      <c r="E41" s="5">
+        <f>B41*D41</f>
+        <v>482.04</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E42" s="5">
+        <f>SUM(E38:E41)</f>
+        <v>482.04</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+    </row>
+    <row r="46" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="3">
+        <f>1+1.5+0.5+0.5+2+1+1+2+0.5+2.5+1.5+2</f>
+        <v>16</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D47" s="21">
+        <v>13.39</v>
+      </c>
+      <c r="E47" s="5">
+        <f>B47*D47</f>
+        <v>214.24</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D48" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" s="5">
+        <f>SUM(E44:E47)</f>
+        <v>214.24</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="55"/>
-      <c r="E37" s="55"/>
-    </row>
-    <row r="38" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="3">
-        <v>15</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="21">
+      <c r="C51" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" s="55"/>
+      <c r="E51" s="55"/>
+    </row>
+    <row r="52" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="3">
+        <f>0.3+1+0.5+2+2+2+5+1+0.5+1+1.5+1.5+1.5+2+7+7+5</f>
+        <v>40.799999999999997</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D53" s="21">
         <v>13.39</v>
       </c>
-      <c r="E39" s="5">
-        <f>B39*D39</f>
-        <v>200.85000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D40" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" s="5">
-        <f>SUM(E36:E39)</f>
-        <v>200.85000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="54" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
-    </row>
-    <row r="44" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="3">
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="21">
+      <c r="E53" s="5">
+        <f>B53*D53</f>
+        <v>546.31200000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D54" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E54" s="5">
+        <f>SUM(E50:E53)</f>
+        <v>546.31200000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C57" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="55"/>
+      <c r="E57" s="55"/>
+    </row>
+    <row r="58" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="3">
+        <v>3</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="21">
         <v>13.39</v>
       </c>
-      <c r="E45" s="5">
-        <f>B45*D45</f>
-        <v>116.49299999999999</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D46" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46" s="5">
-        <f>SUM(E42:E45)</f>
-        <v>116.49299999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C49" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-    </row>
-    <row r="50" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="51" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B51" s="3">
-        <v>24.6</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="21">
-        <v>13.39</v>
-      </c>
-      <c r="E51" s="5">
-        <f>B51*D51</f>
-        <v>329.39400000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D52" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E52" s="5">
-        <f>SUM(E48:E51)</f>
-        <v>329.39400000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C55" s="54" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="55"/>
-      <c r="E55" s="55"/>
-    </row>
-    <row r="56" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B57" s="3">
-        <v>1</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D57" s="21">
-        <v>13.39</v>
-      </c>
-      <c r="E57" s="5">
-        <f>B57*D57</f>
-        <v>13.39</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D58" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E58" s="5">
-        <f>SUM(E54:E57)</f>
-        <v>13.39</v>
+      <c r="E59" s="5">
+        <f>B59*D59</f>
+        <v>40.17</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D60" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" s="5">
+        <f>SUM(E56:E59)</f>
+        <v>40.17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C57:E57"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C17:E17"/>
     <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C30:E30"/>
+    <mergeCell ref="C31:E31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1917,8 +2097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1930,7 +2110,7 @@
   <sheetData>
     <row r="2" spans="1:4" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A2" s="56" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" s="56"/>
       <c r="C2" s="56"/>
@@ -1938,13 +2118,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D3" s="60"/>
     </row>
@@ -1953,11 +2133,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C4" s="57">
         <f>'Precios de unidades de obra'!E7</f>
-        <v>338.625</v>
+        <v>455.40000000000003</v>
       </c>
       <c r="D4" s="58"/>
     </row>
@@ -1966,11 +2146,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C5" s="57">
         <f>'Precios de unidades de obra'!E14</f>
-        <v>96.75</v>
+        <v>202.4</v>
       </c>
       <c r="D5" s="58"/>
     </row>
@@ -1979,11 +2159,11 @@
         <v>1</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C6" s="57">
         <f>'Precios de unidades de obra'!E20</f>
-        <v>638.55000000000007</v>
+        <v>1037.3</v>
       </c>
       <c r="D6" s="58"/>
     </row>
@@ -1992,11 +2172,11 @@
         <v>1</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C7" s="57">
-        <f>'Precios de unidades de obra'!E26</f>
-        <v>715.95</v>
+        <f>'Precios de unidades de obra'!E27</f>
+        <v>2122.46</v>
       </c>
       <c r="D7" s="58"/>
     </row>
@@ -2005,11 +2185,11 @@
         <v>1</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C8" s="57">
-        <f>'Precios de unidades de obra'!E33</f>
-        <v>290.25</v>
+        <f>'Precios de unidades de obra'!E35</f>
+        <v>1369.6</v>
       </c>
       <c r="D8" s="58"/>
     </row>
@@ -2018,11 +2198,11 @@
         <v>1</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C9" s="57">
-        <f>'Precios de unidades de obra'!E40</f>
-        <v>200.85000000000002</v>
+        <f>'Precios de unidades de obra'!E42</f>
+        <v>482.04</v>
       </c>
       <c r="D9" s="58"/>
     </row>
@@ -2031,11 +2211,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C10" s="57">
-        <f>'Precios de unidades de obra'!E46</f>
-        <v>116.49299999999999</v>
+        <f>'Precios de unidades de obra'!E48</f>
+        <v>214.24</v>
       </c>
       <c r="D10" s="58"/>
     </row>
@@ -2044,11 +2224,11 @@
         <v>1</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C11" s="57">
-        <f>'Precios de unidades de obra'!E52</f>
-        <v>329.39400000000001</v>
+        <f>'Precios de unidades de obra'!E54</f>
+        <v>546.31200000000001</v>
       </c>
       <c r="D11" s="58"/>
     </row>
@@ -2057,11 +2237,11 @@
         <v>1</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C12" s="57">
-        <f>'Precios de unidades de obra'!E58</f>
-        <v>13.39</v>
+        <f>'Precios de unidades de obra'!E60</f>
+        <v>40.17</v>
       </c>
       <c r="D12" s="58"/>
     </row>
@@ -2069,57 +2249,57 @@
       <c r="A13" s="24"/>
       <c r="B13" s="25"/>
       <c r="C13" s="26" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D13" s="27">
         <f>SUM(C4:D12)</f>
-        <v>2740.252</v>
+        <v>6469.9219999999996</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="28"/>
       <c r="B14" s="29" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D14" s="31">
-        <f>D13*0.1</f>
-        <v>274.02519999999998</v>
+        <f>D13*0.17</f>
+        <v>1099.8867399999999</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="28"/>
       <c r="B15" s="32"/>
       <c r="C15" s="33" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D15" s="34">
         <f>D13+D14</f>
-        <v>3014.2772</v>
+        <v>7569.8087399999995</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="28"/>
       <c r="B16" s="35"/>
       <c r="C16" s="29" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D16" s="36">
         <f>D13*0.3</f>
-        <v>822.07560000000001</v>
+        <v>1940.9765999999997</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="37"/>
       <c r="B17" s="38"/>
       <c r="C17" s="39" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D17" s="40">
         <f>D15+D16</f>
-        <v>3836.3528000000001</v>
+        <v>9510.7853399999985</v>
       </c>
     </row>
   </sheetData>
@@ -2144,8 +2324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,7 +2337,7 @@
   <sheetData>
     <row r="3" spans="2:7" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B3" s="41" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C3" s="41"/>
     </row>
@@ -2169,11 +2349,11 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C5" s="43">
-        <f>SUM('Presupuesto Interno'!C4:D8)*1.4</f>
-        <v>2912.1749999999997</v>
+        <f>SUM('Presupuesto Interno'!C4:D8)*1.47</f>
+        <v>7625.1251999999995</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50"/>
@@ -2182,31 +2362,31 @@
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="42" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C6" s="43">
-        <f>SUM('Presupuesto Interno'!C9:D12)*1.4</f>
-        <v>924.17780000000005</v>
+        <f>SUM('Presupuesto Interno'!C9:D12)*1.47</f>
+        <v>1885.6601400000002</v>
       </c>
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
     </row>
     <row r="7" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B7" s="44" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C7" s="45">
         <f>SUM(C5:C6)</f>
-        <v>3836.3527999999997</v>
+        <v>9510.7853400000004</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="46" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C8" s="47">
         <f>C7*0.21</f>
-        <v>805.63408799999991</v>
+        <v>1997.2649214</v>
       </c>
       <c r="D8" s="50"/>
       <c r="E8" s="50"/>
@@ -2214,11 +2394,11 @@
     </row>
     <row r="9" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="48" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C9" s="49">
         <f>C7+C8</f>
-        <v>4641.9868879999995</v>
+        <v>11508.0502614</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>